<commit_message>
Find zeta for all paramstudy cases after AF fixes + testing
</commit_message>
<xml_diff>
--- a/ParamStudy/paramStudy.xlsx
+++ b/ParamStudy/paramStudy.xlsx
@@ -15,7 +15,7 @@
     <sheet name="paramStudy" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">paramStudy!$A$1:$O$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">paramStudy!$A$1:$O$67</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -556,10 +556,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -881,13 +883,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O74"/>
+  <dimension ref="A1:Q70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomRight" activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -895,7 +897,7 @@
     <col min="15" max="15" width="9.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -942,7 +944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -983,13 +985,21 @@
         <v>20</v>
       </c>
       <c r="N2" s="1">
-        <v>4.6205999999999997E-2</v>
+        <v>4.4679842708450997E-2</v>
       </c>
       <c r="O2" s="2">
-        <v>6.6992999999999997E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.7018103834118006E-2</v>
+      </c>
+      <c r="P2">
+        <f>B2*40000</f>
+        <v>2000</v>
+      </c>
+      <c r="Q2">
+        <f>IF(M2&lt;P2,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1027,16 +1037,24 @@
         <v>2</v>
       </c>
       <c r="M3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N3" s="1">
-        <v>4.7898999999999997E-3</v>
+        <v>4.9827357117082199E-5</v>
       </c>
       <c r="O3" s="2">
-        <v>6.5685999999999994E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.6505973128707999E-2</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P66" si="0">B3*40000</f>
+        <v>6320</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q66" si="1">IF(M3&lt;P3,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1074,16 +1092,24 @@
         <v>2</v>
       </c>
       <c r="M4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
       <c r="O4" s="2">
-        <v>8.1867999999999996E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.2032248691052106E-2</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1124,13 +1150,21 @@
         <v>18</v>
       </c>
       <c r="N5" s="1">
-        <v>1.5915E-3</v>
+        <v>1.6408694617599999E-3</v>
       </c>
       <c r="O5" s="2">
-        <v>6.6170999999999994E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.5842418935896999E-2</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1168,16 +1202,24 @@
         <v>2</v>
       </c>
       <c r="M6">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
       <c r="O6" s="2">
-        <v>8.1962999999999994E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.2104187282043994E-2</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1215,16 +1257,24 @@
         <v>2</v>
       </c>
       <c r="M7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N7" s="1">
-        <v>4.1634847714850497E-3</v>
+        <v>3.0964981144358601E-3</v>
       </c>
       <c r="O7" s="2">
-        <v>6.5797153907064504E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.5509011066304093E-2</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1262,16 +1312,24 @@
         <v>2</v>
       </c>
       <c r="M8">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N8">
         <v>0</v>
       </c>
       <c r="O8" s="1">
-        <v>8.1839462044513894E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.2026899528789901E-2</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1309,16 +1367,24 @@
         <v>2</v>
       </c>
       <c r="M9">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N9" s="1">
-        <v>4.1634847714850497E-3</v>
+        <v>1.05785357129238E-3</v>
       </c>
       <c r="O9" s="2">
-        <v>6.5797153907064504E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.5963597289343104E-2</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1355,17 +1421,25 @@
       <c r="L10">
         <v>2</v>
       </c>
-      <c r="M10">
-        <v>37</v>
+      <c r="M10" s="3">
+        <v>42</v>
       </c>
       <c r="N10">
         <v>0</v>
       </c>
       <c r="O10" s="1">
-        <v>8.1839462044513894E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.2289093696611804E-2</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1406,13 +1480,21 @@
         <v>20</v>
       </c>
       <c r="N11" s="1">
-        <v>4.2899E-2</v>
+        <v>3.06277572446986E-2</v>
       </c>
       <c r="O11" s="1">
-        <v>6.8806000000000006E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.8905872637899698E-2</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1456,10 +1538,18 @@
         <v>0</v>
       </c>
       <c r="O12" s="1">
-        <v>8.1848000000000004E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.1856040453434697E-2</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1497,16 +1587,24 @@
         <v>2</v>
       </c>
       <c r="M13">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N13" s="1">
-        <v>4.2899E-2</v>
+        <v>4.8765424711410398E-2</v>
       </c>
       <c r="O13" s="1">
-        <v>6.8806000000000006E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.8114865830509005E-2</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1550,10 +1648,18 @@
         <v>0</v>
       </c>
       <c r="O14" s="1">
-        <v>8.1848000000000004E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.2165002003905793E-2</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1594,13 +1700,21 @@
         <v>20</v>
       </c>
       <c r="N15" s="1">
-        <v>4.2899E-2</v>
+        <v>4.2409121757981602E-2</v>
       </c>
       <c r="O15" s="1">
-        <v>6.8806000000000006E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.8698769285851696E-2</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1644,10 +1758,18 @@
         <v>0</v>
       </c>
       <c r="O16" s="1">
-        <v>8.1848000000000004E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.1738741941625406E-2</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1688,13 +1810,21 @@
         <v>20</v>
       </c>
       <c r="N17" s="1">
-        <v>4.2899E-2</v>
+        <v>3.9574950225922098E-2</v>
       </c>
       <c r="O17" s="1">
-        <v>6.8806000000000006E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.8755066598418998E-2</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1738,10 +1868,18 @@
         <v>0</v>
       </c>
       <c r="O18" s="1">
-        <v>8.1848000000000004E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.1775715837462806E-2</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1779,16 +1917,24 @@
         <v>2</v>
       </c>
       <c r="M19">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N19">
         <v>0</v>
       </c>
       <c r="O19" s="1">
-        <v>6.5860000000000002E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.5879367502528402E-2</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1826,16 +1972,24 @@
         <v>2</v>
       </c>
       <c r="M20">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N20">
         <v>0</v>
       </c>
       <c r="O20" s="1">
-        <v>8.1978428089316699E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.1987181199094802E-2</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1873,16 +2027,24 @@
         <v>2</v>
       </c>
       <c r="M21">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="N21">
         <v>0</v>
       </c>
       <c r="O21" s="1">
-        <v>6.5860000000000002E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.5876638210795202E-2</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1920,16 +2082,24 @@
         <v>2</v>
       </c>
       <c r="M22">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="N22">
         <v>0</v>
       </c>
       <c r="O22" s="1">
-        <v>8.1978428089316699E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.2028893682183607E-2</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1973,10 +2143,18 @@
         <v>0</v>
       </c>
       <c r="O23" s="1">
-        <v>6.5860000000000002E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.5910705819195503E-2</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2020,10 +2198,18 @@
         <v>0</v>
       </c>
       <c r="O24" s="1">
-        <v>8.1978428089316699E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.2005875922154803E-2</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2067,10 +2253,18 @@
         <v>0</v>
       </c>
       <c r="O25" s="1">
-        <v>6.5860000000000002E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.6044659893773894E-2</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2114,10 +2308,18 @@
         <v>0</v>
       </c>
       <c r="O26" s="1">
-        <v>8.1978428089316699E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.2060604085601202E-2</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="0"/>
+        <v>6320</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2161,10 +2363,18 @@
         <v>0</v>
       </c>
       <c r="O27" s="1">
-        <v>6.5860000000000002E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.5977604548587906E-2</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2208,10 +2418,18 @@
         <v>0</v>
       </c>
       <c r="O28" s="1">
-        <v>8.1978428089316699E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.2028868352026996E-2</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2255,10 +2473,18 @@
         <v>0</v>
       </c>
       <c r="O29" s="1">
-        <v>6.5860000000000002E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.6099855266332302E-2</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2302,10 +2528,18 @@
         <v>0</v>
       </c>
       <c r="O30" s="1">
-        <v>8.1978428089316699E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.2080299643485996E-2</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2349,10 +2583,18 @@
         <v>0</v>
       </c>
       <c r="O31" s="1">
-        <v>6.5860000000000002E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.58862437242618E-2</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2396,10 +2638,18 @@
         <v>0</v>
       </c>
       <c r="O32" s="1">
-        <v>8.1978428089316699E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.1996833744150496E-2</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2443,10 +2693,18 @@
         <v>0</v>
       </c>
       <c r="O33" s="1">
-        <v>6.5860000000000002E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6.5899528284115202E-2</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2490,10 +2748,18 @@
         <v>0</v>
       </c>
       <c r="O34" s="1">
-        <v>8.1978428089316699E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8.2001707794445503E-2</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2539,8 +2805,16 @@
       <c r="O35" s="1">
         <v>9.3325000000000005E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P35">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2586,8 +2860,16 @@
       <c r="O36" s="1">
         <v>9.7753999999999994E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P36">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2625,16 +2907,24 @@
         <v>2</v>
       </c>
       <c r="M37">
-        <v>24</v>
-      </c>
-      <c r="N37" s="1">
-        <v>4.5373999999999998E-2</v>
+        <v>21</v>
+      </c>
+      <c r="N37" s="4">
+        <v>5.0975006846763801E-2</v>
       </c>
       <c r="O37" s="1">
         <v>9.3325000000000005E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P37">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2672,16 +2962,24 @@
         <v>2</v>
       </c>
       <c r="M38">
-        <v>28</v>
-      </c>
-      <c r="N38" s="1">
-        <v>9.8239E-3</v>
+        <v>27</v>
+      </c>
+      <c r="N38" s="4">
+        <v>5.8956161712017301E-3</v>
       </c>
       <c r="O38" s="1">
         <v>9.7753999999999994E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P38">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2719,16 +3017,24 @@
         <v>2</v>
       </c>
       <c r="M39">
-        <v>24</v>
-      </c>
-      <c r="N39" s="1">
-        <v>4.5373999999999998E-2</v>
+        <v>22</v>
+      </c>
+      <c r="N39" s="4">
+        <v>4.4874672014504201E-2</v>
       </c>
       <c r="O39" s="1">
         <v>9.3325000000000005E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P39">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2766,16 +3072,24 @@
         <v>2</v>
       </c>
       <c r="M40">
-        <v>28</v>
-      </c>
-      <c r="N40" s="1">
-        <v>9.8239E-3</v>
+        <v>26</v>
+      </c>
+      <c r="N40" s="4">
+        <v>1.03819569359855E-2</v>
       </c>
       <c r="O40" s="1">
         <v>9.7753999999999994E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P40">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2815,14 +3129,22 @@
       <c r="M41">
         <v>24</v>
       </c>
-      <c r="N41" s="1">
-        <v>4.5373999999999998E-2</v>
+      <c r="N41" s="4">
+        <v>4.4715112707687001E-2</v>
       </c>
       <c r="O41" s="1">
         <v>9.3325000000000005E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P41">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2862,14 +3184,22 @@
       <c r="M42">
         <v>28</v>
       </c>
-      <c r="N42" s="1">
-        <v>9.8239E-3</v>
+      <c r="N42" s="4">
+        <v>9.5776739104209106E-3</v>
       </c>
       <c r="O42" s="1">
         <v>9.7753999999999994E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P42">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2907,16 +3237,24 @@
         <v>2</v>
       </c>
       <c r="M43">
-        <v>24</v>
-      </c>
-      <c r="N43" s="1">
-        <v>4.5373999999999998E-2</v>
+        <v>22</v>
+      </c>
+      <c r="N43" s="4">
+        <v>4.4874672014572202E-2</v>
       </c>
       <c r="O43" s="1">
         <v>9.3325000000000005E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P43">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2954,16 +3292,24 @@
         <v>2</v>
       </c>
       <c r="M44">
-        <v>28</v>
-      </c>
-      <c r="N44" s="1">
-        <v>9.8239E-3</v>
+        <v>26</v>
+      </c>
+      <c r="N44" s="4">
+        <v>1.03819569359857E-2</v>
       </c>
       <c r="O44" s="1">
         <v>9.7753999999999994E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P44">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3001,16 +3347,24 @@
         <v>2</v>
       </c>
       <c r="M45">
-        <v>24</v>
-      </c>
-      <c r="N45" s="1">
-        <v>4.5373999999999998E-2</v>
+        <v>21</v>
+      </c>
+      <c r="N45" s="4">
+        <v>5.0975006846762601E-2</v>
       </c>
       <c r="O45" s="1">
         <v>9.3325000000000005E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P45">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3048,16 +3402,24 @@
         <v>2</v>
       </c>
       <c r="M46">
-        <v>28</v>
-      </c>
-      <c r="N46" s="1">
-        <v>9.8239E-3</v>
+        <v>27</v>
+      </c>
+      <c r="N46" s="4">
+        <v>5.8956161712018298E-3</v>
       </c>
       <c r="O46" s="1">
         <v>9.7753999999999994E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P46">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3097,14 +3459,22 @@
       <c r="M47">
         <v>24</v>
       </c>
-      <c r="N47" s="1">
-        <v>4.5373999999999998E-2</v>
+      <c r="N47" s="4">
+        <v>4.4526449412279699E-2</v>
       </c>
       <c r="O47" s="1">
         <v>9.3325000000000005E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P47">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3144,14 +3514,22 @@
       <c r="M48">
         <v>28</v>
       </c>
-      <c r="N48" s="1">
-        <v>9.8239E-3</v>
+      <c r="N48" s="4">
+        <v>1.0025364598100901E-2</v>
       </c>
       <c r="O48" s="1">
         <v>9.7753999999999994E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P48">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3191,14 +3569,22 @@
       <c r="M49">
         <v>24</v>
       </c>
-      <c r="N49" s="1">
-        <v>4.5373999999999998E-2</v>
+      <c r="N49" s="4">
+        <v>4.4715112707686903E-2</v>
       </c>
       <c r="O49" s="1">
         <v>9.3325000000000005E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P49">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3238,14 +3624,22 @@
       <c r="M50">
         <v>28</v>
       </c>
-      <c r="N50" s="1">
-        <v>9.8239E-3</v>
+      <c r="N50" s="4">
+        <v>9.5776739104209106E-3</v>
       </c>
       <c r="O50" s="1">
         <v>9.7753999999999994E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P50">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3283,7 +3677,7 @@
         <v>2</v>
       </c>
       <c r="M51">
-        <v>455</v>
+        <v>387</v>
       </c>
       <c r="N51">
         <v>0</v>
@@ -3291,8 +3685,16 @@
       <c r="O51" s="1">
         <v>6.6006999999999996E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P51">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3330,7 +3732,7 @@
         <v>2</v>
       </c>
       <c r="M52">
-        <v>6060</v>
+        <v>6000</v>
       </c>
       <c r="N52">
         <v>0</v>
@@ -3338,8 +3740,16 @@
       <c r="O52" s="1">
         <v>9.8006999999999997E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P52">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3377,7 +3787,7 @@
         <v>2</v>
       </c>
       <c r="M53">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="N53">
         <v>0</v>
@@ -3385,8 +3795,16 @@
       <c r="O53" s="1">
         <v>6.6006999999999996E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P53">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3432,8 +3850,16 @@
       <c r="O54" s="1">
         <v>9.8006999999999997E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P54">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3479,8 +3905,16 @@
       <c r="O55" s="1">
         <v>6.6006999999999996E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P55">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3526,8 +3960,16 @@
       <c r="O56" s="1">
         <v>9.8006999999999997E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P56">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3573,8 +4015,16 @@
       <c r="O57" s="1">
         <v>6.6006999999999996E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P57">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3620,8 +4070,16 @@
       <c r="O58" s="1">
         <v>9.8006999999999997E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P58">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3667,8 +4125,16 @@
       <c r="O59" s="1">
         <v>6.6006999999999996E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P59">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3714,8 +4180,16 @@
       <c r="O60" s="1">
         <v>9.8006999999999997E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P60">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3761,8 +4235,16 @@
       <c r="O61" s="1">
         <v>6.6006999999999996E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P61">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3808,8 +4290,16 @@
       <c r="O62" s="1">
         <v>9.8006999999999997E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P62">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3855,8 +4345,16 @@
       <c r="O63" s="1">
         <v>6.6006999999999996E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P63">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3902,8 +4400,16 @@
       <c r="O64" s="1">
         <v>9.8006999999999997E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P64">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3949,8 +4455,16 @@
       <c r="O65" s="1">
         <v>6.6006999999999996E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P65">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3996,8 +4510,16 @@
       <c r="O66" s="1">
         <v>9.8006999999999997E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P66">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4044,24 +4566,24 @@
         <v>6.6773552202674294E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68">
-        <v>1.4999999999999999E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68">
-        <v>16.5</v>
+        <v>60</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G68">
         <v>6.6000000000000003E-2</v>
@@ -4082,33 +4604,41 @@
         <v>2</v>
       </c>
       <c r="M68">
-        <v>20</v>
-      </c>
-      <c r="N68" s="1">
-        <v>5.7195171241138799E-2</v>
-      </c>
-      <c r="O68" s="2">
-        <v>6.6773552202674294E-2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+        <v>455</v>
+      </c>
+      <c r="N68">
+        <v>0</v>
+      </c>
+      <c r="O68" s="1">
+        <v>6.6006999999999996E-2</v>
+      </c>
+      <c r="P68">
+        <f t="shared" ref="P68:P69" si="2">B68*40000</f>
+        <v>200</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" ref="Q68:Q69" si="3">IF(M68&lt;P68,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69">
-        <v>0.158</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69">
-        <v>16.5</v>
+        <v>60</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G69">
         <v>6.6000000000000003E-2</v>
@@ -4129,33 +4659,41 @@
         <v>2</v>
       </c>
       <c r="M69">
-        <v>20</v>
-      </c>
-      <c r="N69" s="1">
-        <v>5.7195171241138799E-2</v>
-      </c>
-      <c r="O69" s="2">
-        <v>6.6773552202674294E-2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+        <v>455</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69" s="1">
+        <v>6.6006999999999996E-2</v>
+      </c>
+      <c r="P69">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="Q69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70">
-        <v>0.5</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70">
-        <v>16.5</v>
+        <v>76.5</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G70">
         <v>6.6000000000000003E-2</v>
@@ -4176,205 +4714,25 @@
         <v>2</v>
       </c>
       <c r="M70">
-        <v>20</v>
-      </c>
-      <c r="N70" s="1">
-        <v>5.7195171241138799E-2</v>
-      </c>
-      <c r="O70" s="2">
-        <v>6.6773552202674294E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71">
-        <v>0.05</v>
-      </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
-      <c r="D71">
-        <v>4.2</v>
-      </c>
-      <c r="E71">
-        <v>1</v>
-      </c>
-      <c r="F71">
-        <v>1</v>
-      </c>
-      <c r="G71">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="H71">
-        <v>0</v>
-      </c>
-      <c r="I71">
-        <v>0</v>
-      </c>
-      <c r="J71">
-        <v>2</v>
-      </c>
-      <c r="K71">
-        <v>1</v>
-      </c>
-      <c r="L71">
-        <v>2</v>
-      </c>
-      <c r="M71">
-        <v>23</v>
-      </c>
-      <c r="N71" s="1">
-        <v>1.4579999999999999E-2</v>
-      </c>
-      <c r="O71" s="2">
-        <v>8.1610000000000002E-2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="B72">
-        <v>0.05</v>
-      </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
-      <c r="D72">
-        <v>35.5</v>
-      </c>
-      <c r="E72">
-        <v>1</v>
-      </c>
-      <c r="F72">
-        <v>1</v>
-      </c>
-      <c r="G72">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="H72">
-        <v>0</v>
-      </c>
-      <c r="I72">
-        <v>0</v>
-      </c>
-      <c r="J72">
-        <v>2</v>
-      </c>
-      <c r="K72">
-        <v>1</v>
-      </c>
-      <c r="L72">
-        <v>2</v>
-      </c>
-      <c r="M72">
-        <v>130</v>
-      </c>
-      <c r="N72">
-        <v>0</v>
-      </c>
-      <c r="O72" s="2">
-        <v>8.1977999999999995E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="B73">
-        <v>0.05</v>
-      </c>
-      <c r="C73">
-        <v>1</v>
-      </c>
-      <c r="D73">
-        <v>50</v>
-      </c>
-      <c r="E73">
-        <v>1</v>
-      </c>
-      <c r="F73">
-        <v>1</v>
-      </c>
-      <c r="G73">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="H73">
-        <v>0</v>
-      </c>
-      <c r="I73">
-        <v>0</v>
-      </c>
-      <c r="J73">
-        <v>2</v>
-      </c>
-      <c r="K73">
-        <v>1</v>
-      </c>
-      <c r="L73">
-        <v>2</v>
-      </c>
-      <c r="M73">
-        <v>335</v>
-      </c>
-      <c r="N73">
-        <v>0</v>
-      </c>
-      <c r="O73" s="2">
-        <v>8.1942000000000001E-2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="B74">
-        <v>0.05</v>
-      </c>
-      <c r="C74">
-        <v>1</v>
-      </c>
-      <c r="D74">
-        <v>76.5</v>
-      </c>
-      <c r="E74">
-        <v>1</v>
-      </c>
-      <c r="F74">
-        <v>1</v>
-      </c>
-      <c r="G74">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="H74">
-        <v>0</v>
-      </c>
-      <c r="I74">
-        <v>0</v>
-      </c>
-      <c r="J74">
-        <v>2</v>
-      </c>
-      <c r="K74">
-        <v>1</v>
-      </c>
-      <c r="L74">
-        <v>2</v>
-      </c>
-      <c r="M74">
-        <v>1680</v>
-      </c>
-      <c r="N74">
-        <v>0</v>
-      </c>
-      <c r="O74" s="2">
-        <v>8.2138000000000003E-2</v>
+        <v>455</v>
+      </c>
+      <c r="N70">
+        <v>0</v>
+      </c>
+      <c r="O70" s="1">
+        <v>6.6006999999999996E-2</v>
+      </c>
+      <c r="P70">
+        <f t="shared" ref="P70" si="4">B70*40000</f>
+        <v>200</v>
+      </c>
+      <c r="Q70">
+        <f t="shared" ref="Q70" si="5">IF(M70&lt;P70,1,0)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O74"/>
+  <autoFilter ref="A1:O67"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
lots of stuff - just a backup
</commit_message>
<xml_diff>
--- a/ParamStudy/paramStudy.xlsx
+++ b/ParamStudy/paramStudy.xlsx
@@ -15,7 +15,7 @@
     <sheet name="paramStudy" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">paramStudy!$A$1:$O$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">paramStudy!$A$1:$O$66</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -884,13 +884,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q82"/>
+  <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M36" sqref="M36"/>
+      <selection pane="bottomRight" activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4085,7 +4085,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>5.0000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -4128,11 +4128,11 @@
       </c>
       <c r="P59">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="Q59">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.35">
@@ -4140,7 +4140,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>5.0000000000000001E-3</v>
+        <v>0.158</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -4183,11 +4183,11 @@
       </c>
       <c r="P60">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>6320</v>
       </c>
       <c r="Q60">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.35">
@@ -4195,7 +4195,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>5.0000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -4238,11 +4238,11 @@
       </c>
       <c r="P61">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="Q61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.35">
@@ -4250,7 +4250,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>5.0000000000000001E-3</v>
+        <v>0.158</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -4293,11 +4293,11 @@
       </c>
       <c r="P62">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>6320</v>
       </c>
       <c r="Q62">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.35">
@@ -4305,7 +4305,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>5.0000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -4348,11 +4348,11 @@
       </c>
       <c r="P63">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="Q63">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.35">
@@ -4360,7 +4360,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>5.0000000000000001E-3</v>
+        <v>0.158</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -4403,11 +4403,11 @@
       </c>
       <c r="P64">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>6320</v>
       </c>
       <c r="Q64">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.35">
@@ -4415,7 +4415,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>5.0000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -4458,11 +4458,11 @@
       </c>
       <c r="P65">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="Q65">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.35">
@@ -4470,7 +4470,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>5.0000000000000001E-3</v>
+        <v>0.158</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -4513,676 +4513,15 @@
       </c>
       <c r="P66">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>6320</v>
       </c>
       <c r="Q66">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="B67">
-        <v>0.5</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-      <c r="D67">
-        <v>60</v>
-      </c>
-      <c r="E67">
-        <v>10</v>
-      </c>
-      <c r="F67">
-        <v>2</v>
-      </c>
-      <c r="G67">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="H67">
-        <v>0</v>
-      </c>
-      <c r="I67">
-        <v>0</v>
-      </c>
-      <c r="J67">
-        <v>2</v>
-      </c>
-      <c r="K67">
-        <v>1</v>
-      </c>
-      <c r="L67">
-        <v>2</v>
-      </c>
-      <c r="M67">
-        <v>387</v>
-      </c>
-      <c r="N67" s="1"/>
-      <c r="O67" s="2"/>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="B68">
-        <v>0.5</v>
-      </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
-      <c r="D68">
-        <v>60</v>
-      </c>
-      <c r="E68">
-        <v>10</v>
-      </c>
-      <c r="F68">
-        <v>2</v>
-      </c>
-      <c r="G68">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="H68">
-        <v>0</v>
-      </c>
-      <c r="I68">
-        <v>0</v>
-      </c>
-      <c r="J68">
-        <v>2</v>
-      </c>
-      <c r="K68">
-        <v>1</v>
-      </c>
-      <c r="L68">
-        <v>2</v>
-      </c>
-      <c r="M68">
-        <v>6000</v>
-      </c>
-      <c r="O68" s="1"/>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="B69">
-        <v>0.5</v>
-      </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
-      <c r="D69">
-        <v>60</v>
-      </c>
-      <c r="E69">
-        <v>10</v>
-      </c>
-      <c r="F69">
-        <v>6</v>
-      </c>
-      <c r="G69">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
-      <c r="I69">
-        <v>0</v>
-      </c>
-      <c r="J69">
-        <v>2</v>
-      </c>
-      <c r="K69">
-        <v>1</v>
-      </c>
-      <c r="L69">
-        <v>2</v>
-      </c>
-      <c r="M69">
-        <v>450</v>
-      </c>
-      <c r="O69" s="1"/>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A70">
-        <v>69</v>
-      </c>
-      <c r="B70">
-        <v>0.5</v>
-      </c>
-      <c r="C70">
-        <v>1</v>
-      </c>
-      <c r="D70">
-        <v>60</v>
-      </c>
-      <c r="E70">
-        <v>10</v>
-      </c>
-      <c r="F70">
-        <v>6</v>
-      </c>
-      <c r="G70">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-      <c r="I70">
-        <v>0</v>
-      </c>
-      <c r="J70">
-        <v>2</v>
-      </c>
-      <c r="K70">
-        <v>1</v>
-      </c>
-      <c r="L70">
-        <v>2</v>
-      </c>
-      <c r="M70">
-        <v>6060</v>
-      </c>
-      <c r="O70" s="1"/>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71">
-        <v>0.5</v>
-      </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
-      <c r="D71">
-        <v>60</v>
-      </c>
-      <c r="E71">
-        <v>0.1</v>
-      </c>
-      <c r="F71">
-        <v>2</v>
-      </c>
-      <c r="G71">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="H71">
-        <v>0</v>
-      </c>
-      <c r="I71">
-        <v>0</v>
-      </c>
-      <c r="J71">
-        <v>2</v>
-      </c>
-      <c r="K71">
-        <v>1</v>
-      </c>
-      <c r="L71">
-        <v>2</v>
-      </c>
-      <c r="M71">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="B72">
-        <v>0.5</v>
-      </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
-      <c r="D72">
-        <v>60</v>
-      </c>
-      <c r="E72">
-        <v>0.1</v>
-      </c>
-      <c r="F72">
-        <v>2</v>
-      </c>
-      <c r="G72">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="H72">
-        <v>0</v>
-      </c>
-      <c r="I72">
-        <v>0</v>
-      </c>
-      <c r="J72">
-        <v>2</v>
-      </c>
-      <c r="K72">
-        <v>1</v>
-      </c>
-      <c r="L72">
-        <v>2</v>
-      </c>
-      <c r="M72">
-        <v>6060</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="B73">
-        <v>0.5</v>
-      </c>
-      <c r="C73">
-        <v>1</v>
-      </c>
-      <c r="D73">
-        <v>60</v>
-      </c>
-      <c r="E73">
-        <v>0.1</v>
-      </c>
-      <c r="F73">
-        <v>6</v>
-      </c>
-      <c r="G73">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="H73">
-        <v>0</v>
-      </c>
-      <c r="I73">
-        <v>0</v>
-      </c>
-      <c r="J73">
-        <v>2</v>
-      </c>
-      <c r="K73">
-        <v>1</v>
-      </c>
-      <c r="L73">
-        <v>2</v>
-      </c>
-      <c r="M73">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="B74">
-        <v>0.5</v>
-      </c>
-      <c r="C74">
-        <v>1</v>
-      </c>
-      <c r="D74">
-        <v>60</v>
-      </c>
-      <c r="E74">
-        <v>0.1</v>
-      </c>
-      <c r="F74">
-        <v>6</v>
-      </c>
-      <c r="G74">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="H74">
-        <v>0</v>
-      </c>
-      <c r="I74">
-        <v>0</v>
-      </c>
-      <c r="J74">
-        <v>2</v>
-      </c>
-      <c r="K74">
-        <v>1</v>
-      </c>
-      <c r="L74">
-        <v>2</v>
-      </c>
-      <c r="M74">
-        <v>6060</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="B75">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C75">
-        <v>1</v>
-      </c>
-      <c r="D75">
-        <v>60</v>
-      </c>
-      <c r="E75">
-        <v>10</v>
-      </c>
-      <c r="F75">
-        <v>2</v>
-      </c>
-      <c r="G75">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="H75">
-        <v>0</v>
-      </c>
-      <c r="I75">
-        <v>0</v>
-      </c>
-      <c r="J75">
-        <v>2</v>
-      </c>
-      <c r="K75">
-        <v>1</v>
-      </c>
-      <c r="L75">
-        <v>2</v>
-      </c>
-      <c r="M75">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A76">
-        <v>75</v>
-      </c>
-      <c r="B76">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C76">
-        <v>1</v>
-      </c>
-      <c r="D76">
-        <v>60</v>
-      </c>
-      <c r="E76">
-        <v>10</v>
-      </c>
-      <c r="F76">
-        <v>2</v>
-      </c>
-      <c r="G76">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="H76">
-        <v>0</v>
-      </c>
-      <c r="I76">
-        <v>0</v>
-      </c>
-      <c r="J76">
-        <v>2</v>
-      </c>
-      <c r="K76">
-        <v>1</v>
-      </c>
-      <c r="L76">
-        <v>2</v>
-      </c>
-      <c r="M76">
-        <v>6060</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="B77">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C77">
-        <v>1</v>
-      </c>
-      <c r="D77">
-        <v>60</v>
-      </c>
-      <c r="E77">
-        <v>10</v>
-      </c>
-      <c r="F77">
-        <v>6</v>
-      </c>
-      <c r="G77">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="H77">
-        <v>0</v>
-      </c>
-      <c r="I77">
-        <v>0</v>
-      </c>
-      <c r="J77">
-        <v>2</v>
-      </c>
-      <c r="K77">
-        <v>1</v>
-      </c>
-      <c r="L77">
-        <v>2</v>
-      </c>
-      <c r="M77">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C78">
-        <v>1</v>
-      </c>
-      <c r="D78">
-        <v>60</v>
-      </c>
-      <c r="E78">
-        <v>10</v>
-      </c>
-      <c r="F78">
-        <v>6</v>
-      </c>
-      <c r="G78">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="H78">
-        <v>0</v>
-      </c>
-      <c r="I78">
-        <v>0</v>
-      </c>
-      <c r="J78">
-        <v>2</v>
-      </c>
-      <c r="K78">
-        <v>1</v>
-      </c>
-      <c r="L78">
-        <v>2</v>
-      </c>
-      <c r="M78">
-        <v>6060</v>
-      </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="B79">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C79">
-        <v>1</v>
-      </c>
-      <c r="D79">
-        <v>60</v>
-      </c>
-      <c r="E79">
-        <v>0.1</v>
-      </c>
-      <c r="F79">
-        <v>2</v>
-      </c>
-      <c r="G79">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="H79">
-        <v>0</v>
-      </c>
-      <c r="I79">
-        <v>0</v>
-      </c>
-      <c r="J79">
-        <v>2</v>
-      </c>
-      <c r="K79">
-        <v>1</v>
-      </c>
-      <c r="L79">
-        <v>2</v>
-      </c>
-      <c r="M79">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A80">
-        <v>79</v>
-      </c>
-      <c r="B80">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C80">
-        <v>1</v>
-      </c>
-      <c r="D80">
-        <v>60</v>
-      </c>
-      <c r="E80">
-        <v>0.1</v>
-      </c>
-      <c r="F80">
-        <v>2</v>
-      </c>
-      <c r="G80">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="H80">
-        <v>0</v>
-      </c>
-      <c r="I80">
-        <v>0</v>
-      </c>
-      <c r="J80">
-        <v>2</v>
-      </c>
-      <c r="K80">
-        <v>1</v>
-      </c>
-      <c r="L80">
-        <v>2</v>
-      </c>
-      <c r="M80">
-        <v>6060</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A81">
-        <v>80</v>
-      </c>
-      <c r="B81">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C81">
-        <v>1</v>
-      </c>
-      <c r="D81">
-        <v>60</v>
-      </c>
-      <c r="E81">
-        <v>0.1</v>
-      </c>
-      <c r="F81">
-        <v>6</v>
-      </c>
-      <c r="G81">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="H81">
-        <v>0</v>
-      </c>
-      <c r="I81">
-        <v>0</v>
-      </c>
-      <c r="J81">
-        <v>2</v>
-      </c>
-      <c r="K81">
-        <v>1</v>
-      </c>
-      <c r="L81">
-        <v>2</v>
-      </c>
-      <c r="M81">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A82">
-        <v>81</v>
-      </c>
-      <c r="B82">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C82">
-        <v>1</v>
-      </c>
-      <c r="D82">
-        <v>60</v>
-      </c>
-      <c r="E82">
-        <v>0.1</v>
-      </c>
-      <c r="F82">
-        <v>6</v>
-      </c>
-      <c r="G82">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="H82">
-        <v>0</v>
-      </c>
-      <c r="I82">
-        <v>0</v>
-      </c>
-      <c r="J82">
-        <v>2</v>
-      </c>
-      <c r="K82">
-        <v>1</v>
-      </c>
-      <c r="L82">
-        <v>2</v>
-      </c>
-      <c r="M82">
-        <v>6060</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O67"/>
+  <autoFilter ref="A1:O66"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>